<commit_message>
[refs #1] - Dropdown column added.
</commit_message>
<xml_diff>
--- a/Resident_File.xlsx
+++ b/Resident_File.xlsx
@@ -7,12 +7,16 @@
   </bookViews>
   <sheets>
     <sheet name="TEST_SHEET" r:id="rId3" sheetId="1"/>
+    <sheet name="List_reference_hidden_sheet" r:id="rId4" sheetId="2"/>
   </sheets>
+  <definedNames>
+    <definedName name="HiddenList">List_reference_hidden_sheet!$A$2:$A$9</definedName>
+  </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>NAME</t>
   </si>
@@ -30,6 +34,33 @@
   </si>
   <si>
     <t>NID</t>
+  </si>
+  <si>
+    <t>Cities</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>Kolkata</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>Asam</t>
+  </si>
+  <si>
+    <t>Udisha</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>Panjab</t>
+  </si>
+  <si>
+    <t>Shilong</t>
   </si>
   <si>
     <t>Name0</t>
@@ -262,202 +293,264 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E2" t="n">
         <v>30.0</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="E3" t="n">
         <v>31.0</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E4" t="n">
         <v>32.0</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E5" t="n">
         <v>33.0</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="E6" t="n">
         <v>34.0</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E7" t="n">
         <v>35.0</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="E8" t="n">
         <v>36.0</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E9" t="n">
         <v>37.0</v>
       </c>
       <c r="F9" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="E10" t="n">
         <v>38.0</v>
       </c>
       <c r="F10" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E11" t="n">
         <v>39.0</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" sqref="G2:G9" allowBlank="true" errorStyle="stop">
+      <formula1>HiddenList</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="31.25" customWidth="true"/>
+    <col min="2" max="2" width="31.25" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>